<commit_message>
faltan las descripciones de las cosas
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-21-Catálogo de decisiones estratégicas.xlsx
+++ b/HT-6/Optica BAC-21-Catálogo de decisiones estratégicas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4342948A-B29E-F648-BDB4-16A19DC253F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453128C1-028C-3547-A23E-F3601E313874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="500" windowWidth="19840" windowHeight="14920" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="28800" yWindow="-6780" windowWidth="38400" windowHeight="21100" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-21" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -60,26 +60,137 @@
     <t>BAC-21 Catálogo de decisiones estratégicas (propuesta de valor)</t>
   </si>
   <si>
-    <t>Establecer nuevas alianzas con proveedores en aras de ampliar el catalogo de productos</t>
-  </si>
-  <si>
-    <t>Abrir nuevos puntos de venta a nivel nacional</t>
-  </si>
-  <si>
-    <t>Desarrollar actividades de responsabilidad ambiental</t>
-  </si>
-  <si>
-    <t>Hacer promociones de productos disminuyendo los precios si se compran en paquete</t>
-  </si>
-  <si>
-    <t>Hacer campañas de publicidad hacia prospectos de clientes</t>
+    <t>Establecer nuevas alianzas con proveedores</t>
+  </si>
+  <si>
+    <t>Nuestro catálogo debe ser más amplio y actuar con base en la demanda</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>Debemos abrir nuevos puntos de venta a nivel nacional</t>
+  </si>
+  <si>
+    <t>Estudio de mercado</t>
+  </si>
+  <si>
+    <t>Optimización de procesos de importación</t>
+  </si>
+  <si>
+    <t>Negocio</t>
+  </si>
+  <si>
+    <t>&gt; encuestas, análisis de ventas, análisis de peticiones ? Del cliente</t>
+  </si>
+  <si>
+    <t>Estudio de mercado, enfocado a la ubicación de nuestros clientes</t>
+  </si>
+  <si>
+    <t>&gt; lo que dijo jorge de llevar a bogota</t>
+  </si>
+  <si>
+    <t>&gt; preguntarle a los clientes de donde vienen, preguntar en que lugar tendríamos buen recibimiento</t>
+  </si>
+  <si>
+    <t>Publicitarnos en los nuevos puntos de venta</t>
+  </si>
+  <si>
+    <t>Logística de aprovisionamiento</t>
+  </si>
+  <si>
+    <t>Financiero</t>
+  </si>
+  <si>
+    <t>Buscar arriendos en lugares reconocibles y frecuentados</t>
+  </si>
+  <si>
+    <t>&gt; arrendar en centros comerciales y en lugares exclusivos primero, inversion en empleados y overall buena presencia de nuestro establecimiento</t>
+  </si>
+  <si>
+    <t>Nuestra marca debe ser amigable con el cliente</t>
+  </si>
+  <si>
+    <t>Buscar metodologías amigables con el medio ambiente y visibilizarlas</t>
+  </si>
+  <si>
+    <t>Cuidar la imagen y buen estado de nuestros locales</t>
+  </si>
+  <si>
+    <t>&gt; contratar servicios de limpieza, contratar un diseñador que nos oriente a tener un ambiente agradable para las ventas?</t>
+  </si>
+  <si>
+    <t>Tener una estrategia de mercado orientada a hacer sentir al cliente cómodo</t>
+  </si>
+  <si>
+    <t>&gt; tener un asesor que  asesoria de imagen, empleados vestidos elegantes para mostrar imagen institucional</t>
+  </si>
+  <si>
+    <t>&gt; Segmentar el mercado de acuerdo con nuestros estudios para tener una mejor cercanía, mejor lenguaje, buscar qué es trendy</t>
+  </si>
+  <si>
+    <t>Estratégico</t>
+  </si>
+  <si>
+    <t>&gt; no estar atado a solo comprarle un proveedor</t>
+  </si>
+  <si>
+    <t>No tener ninguna afiliación de compromiso con ningún proveedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No comprar al por mayor sino de acuerdo a la demanda, </t>
+  </si>
+  <si>
+    <t>Estrategico</t>
+  </si>
+  <si>
+    <t>Estratético</t>
+  </si>
+  <si>
+    <t>Buscar medios para generar cercanía con el cliente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +210,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -114,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -175,23 +291,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -212,6 +342,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,42 +684,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="56.5" customWidth="1"/>
+    <col min="5" max="5" width="75.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -579,199 +736,293 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="7"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A9" s="7"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="8"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F10" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A13" s="7"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.15">
       <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="8"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="F14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A17" s="7"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.15">
       <c r="A18" s="7"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="7"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="7"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="8"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A15:A18"/>
     <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A24:A28"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Optica BAC-21-Catálogo de decisiones estratégicas.xlsx
</commit_message>
<xml_diff>
--- a/HT-6/Optica BAC-21-Catálogo de decisiones estratégicas.xlsx
+++ b/HT-6/Optica BAC-21-Catálogo de decisiones estratégicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4DB505-7AF2-ED47-9457-67209FE46D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0CF034-1417-A74A-840D-0ED682709EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-6780" windowWidth="38400" windowHeight="21100" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -202,6 +202,45 @@
   </si>
   <si>
     <t>La empresa debe velar por la integridad de los empleados, teniendo en cuenta todas las labores que desempeñan se les otorgarán beneficios como cajas de compensación y afiliaciones obligatorias dentro de un contrato laboral. Todo empleado será contratado mediante contrato laboral.</t>
+  </si>
+  <si>
+    <t>Debemos ampliar nuestros canales de distribución para incluir canales digitales</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>Abrir un nuevo canal de relacionamiento digital con el cliente</t>
+  </si>
+  <si>
+    <t>Abrir un nuevo canal de distribución a domicilio</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>Buscar mantener un sistema informático que permita la venta online de nuestros productos</t>
+  </si>
+  <si>
+    <t>Mediante una plataforma tipo marketplace, la empresa debe comercializar todos los productos que tiene disponibles. Esto con el fin de maximizar las ventas</t>
+  </si>
+  <si>
+    <t>La empresa debe empezar a relacionarse con el cliente digital, para poder exponer todos los productos de forma que las transacciones online sean una parte importante de las ventas</t>
+  </si>
+  <si>
+    <t>La empresa debe encargarse de conseguir un intermediario que realice los envíos de los pedidos</t>
+  </si>
+  <si>
+    <t>Certificación de calidad de productos transformados</t>
+  </si>
+  <si>
+    <t>La empresa debe certificar que los pedidos se realicen cumplan los estándares de calidad de un producto físico, sin necesidad de revisión manual de cada producto. Es decir, la empresa solo será un intermediario entre los proveedores y los clientes, ganando una comisión por ventas en línea.</t>
+  </si>
+  <si>
+    <t>D18</t>
   </si>
 </sst>
 </file>
@@ -334,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -373,6 +412,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -689,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="118" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="118" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -971,36 +1013,70 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+    <row r="20" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.15">
+      <c r="A21" s="16"/>
+      <c r="B21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.15">
+      <c r="A22" s="16"/>
+      <c r="B22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.15">
+      <c r="A23" s="16"/>
+      <c r="B23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="14"/>
+      <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1034,12 +1110,20 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A29" s="14"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>